<commit_message>
tests: Update test files
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model1_input_valid_6.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model1_input_valid_6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -475,8 +475,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -529,7 +529,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2773,7 +2773,7 @@
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>